<commit_message>
Added unit tests for TapeWriter, added a NotedbUserError
</commit_message>
<xml_diff>
--- a/notedb/tests/test_files/test_template.xlsx
+++ b/notedb/tests/test_files/test_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey\git\notedb\tests\test_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jayates\git\notedb\notedb\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="10875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="10872" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>BPO</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Calc</t>
   </si>
   <si>
-    <t>PropAddr</t>
-  </si>
-  <si>
-    <t>PropCity</t>
-  </si>
-  <si>
-    <t>PropState</t>
-  </si>
-  <si>
-    <t>PropZip</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -396,33 +393,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -434,48 +431,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>Sheet1!C2</f>
+        <f>Sheet1!A2</f>
         <v>0</v>
       </c>
       <c r="B2">
-        <f>Sheet1!D2</f>
+        <f>Sheet1!B2</f>
         <v>0</v>
       </c>
       <c r="C2">
-        <f>2*B2</f>
+        <f>A2*B2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>Sheet1!C3</f>
+        <f>Sheet1!A3</f>
         <v>0</v>
       </c>
       <c r="B3">
-        <f>Sheet1!D3</f>
+        <f>Sheet1!B3</f>
         <v>0</v>
       </c>
       <c r="C3">
-        <f>2*B3</f>
+        <f>A3*B3</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>